<commit_message>
Ubah default variables, dan object names
</commit_message>
<xml_diff>
--- a/AutomationPracticeForm/NewCase01Data.xlsx
+++ b/AutomationPracticeForm/NewCase01Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Lawrencon\Interview\case01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Lawencon\Interview\Fix\case01\AutomationPracticeForm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAFFD4C9-6099-4A8F-B555-2CC862A57266}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671F3082-288E-4698-B897-E3A0BC966B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2124" yWindow="2124" windowWidth="17112" windowHeight="8796" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Case01-1-N1" sheetId="2" r:id="rId1"/>
@@ -738,7 +738,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>